<commit_message>
IPA forsøk 2, planlegging
</commit_message>
<xml_diff>
--- a/ipa/bryggeskjema.xlsx
+++ b/ipa/bryggeskjema.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Bryggedato</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Gjær</t>
   </si>
   <si>
-    <t>3 pk</t>
-  </si>
-  <si>
     <t>Mesk</t>
   </si>
   <si>
@@ -160,19 +157,10 @@
     <t>Mesk i 15 min på 72 grader</t>
   </si>
   <si>
-    <t>Kokekar</t>
-  </si>
-  <si>
-    <t>Meskekar</t>
-  </si>
-  <si>
-    <t>oppvarming</t>
-  </si>
-  <si>
-    <t>Justert</t>
-  </si>
-  <si>
-    <t>(3liter kaldt vann)</t>
+    <t>6 pk</t>
+  </si>
+  <si>
+    <t>(evt. 2 hvis starter)</t>
   </si>
 </sst>
 </file>
@@ -570,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +569,7 @@
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -590,7 +578,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -622,7 +610,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -631,10 +619,10 @@
       </c>
       <c r="B6">
         <f>B7+B17*B16+B18</f>
-        <v>72.5</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -643,10 +631,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>62.5</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -703,7 +691,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -711,7 +699,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -719,7 +707,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -741,11 +729,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22">
-        <f>6.9*2.5</f>
-        <v>17.25</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -753,11 +740,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23">
-        <f>0.95*2.5</f>
-        <v>2.375</v>
+        <v>1.5</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -765,11 +751,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24">
-        <f>2.5*0.95</f>
-        <v>2.375</v>
+        <v>1.5</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -780,8 +765,7 @@
         <v>19</v>
       </c>
       <c r="B25">
-        <f>0.75*2.5</f>
-        <v>1.875</v>
+        <v>1.2</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -789,11 +773,11 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <f>SUM(B22:B25)</f>
-        <v>23.875</v>
+        <v>15.2</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -823,14 +807,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>14</v>
       </c>
       <c r="C30">
-        <f>22*2.5</f>
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D30" s="3">
         <v>60</v>
@@ -838,14 +821,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>6</v>
       </c>
       <c r="C31">
-        <f>50*2.5</f>
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="D31" s="3">
         <v>60</v>
@@ -853,101 +835,95 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>6</v>
       </c>
       <c r="C32">
-        <f>60*2.5</f>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D32" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>6</v>
       </c>
       <c r="C33">
-        <f>60*2.5</f>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D33" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>6</v>
       </c>
       <c r="C34">
-        <f>45*2.5</f>
-        <v>112.5</v>
+        <v>50</v>
       </c>
       <c r="D34" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>14</v>
       </c>
       <c r="C35">
-        <f>45*2.5</f>
-        <v>112.5</v>
+        <v>70</v>
       </c>
       <c r="D35" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>14</v>
       </c>
       <c r="C36">
-        <f>50*2.5</f>
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
         <v>38</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37">
+        <v>100</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C37">
-        <f>50*2.5</f>
-        <v>125</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>2</v>
       </c>
@@ -955,107 +931,73 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>26</v>
-      </c>
-      <c r="D44" t="s">
-        <v>51</v>
-      </c>
-      <c r="S44">
-        <f>P46-61</f>
-        <v>31.4236875</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>27</v>
       </c>
       <c r="B45">
         <f>3.1296*B26</f>
-        <v>74.719200000000001</v>
+        <v>47.569919999999996</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45">
-        <f>46+15+3</f>
-        <v>64</v>
-      </c>
-      <c r="E45" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B46">
         <f>B6+0.8345*B26-B45</f>
-        <v>17.704487499999999</v>
+        <v>15.11448</v>
       </c>
       <c r="C46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>29</v>
       </c>
-      <c r="O46" t="s">
+      <c r="B47">
+        <f>SUM(B45:B46)</f>
+        <v>62.684399999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P46">
-        <f>SUM(B45:B46)</f>
-        <v>92.4236875</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="M47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>31</v>
-      </c>
-      <c r="M48" t="s">
-        <v>48</v>
-      </c>
-      <c r="O48">
-        <f>P46/2</f>
-        <v>46.21184375</v>
-      </c>
-      <c r="P48">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>46</v>
-      </c>
-      <c r="M49" t="s">
-        <v>49</v>
-      </c>
-      <c r="O49">
-        <f>P46/2</f>
-        <v>46.21184375</v>
-      </c>
-      <c r="P49">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>